<commit_message>
- Modification of VARS
</commit_message>
<xml_diff>
--- a/Docu/UHA.xlsx
+++ b/Docu/UHA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="0" windowWidth="9390" windowHeight="1185" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="0" windowWidth="9390" windowHeight="1185" firstSheet="1" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="UHA meas values" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,9 @@
     <sheet name="PTC sensor" sheetId="8" r:id="rId9"/>
     <sheet name="Energy VARs" sheetId="9" r:id="rId10"/>
     <sheet name="Energy VARS 2" sheetId="10" r:id="rId11"/>
+    <sheet name="BTL protocol" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -211,7 +211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="528">
   <si>
     <t>dec</t>
   </si>
@@ -1651,13 +1651,194 @@
   </si>
   <si>
     <t>VAR_CONS_TODAY_10WH</t>
+  </si>
+  <si>
+    <t>Frame Format</t>
+  </si>
+  <si>
+    <t>B0</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>msgId</t>
+  </si>
+  <si>
+    <t>Command specific</t>
+  </si>
+  <si>
+    <t>0x11</t>
+  </si>
+  <si>
+    <t>0x12</t>
+  </si>
+  <si>
+    <t>0x13</t>
+  </si>
+  <si>
+    <t>0x14</t>
+  </si>
+  <si>
+    <t>Init Msg</t>
+  </si>
+  <si>
+    <t>Segment Msg</t>
+  </si>
+  <si>
+    <t>Segment Data (4 bytes)</t>
+  </si>
+  <si>
+    <t>BlockNum</t>
+  </si>
+  <si>
+    <t>SegmentNum</t>
+  </si>
+  <si>
+    <t>Finalize Msg</t>
+  </si>
+  <si>
+    <t>Confirm Msg</t>
+  </si>
+  <si>
+    <t>ConfirmCode</t>
+  </si>
+  <si>
+    <t>HWID (Uint16)</t>
+  </si>
+  <si>
+    <t>Total size (Uint32)</t>
+  </si>
+  <si>
+    <t>Total Rec Size (Uint32)</t>
+  </si>
+  <si>
+    <t>Total Sent Size (Uint32)</t>
+  </si>
+  <si>
+    <t>BlockEnd (Bool)</t>
+  </si>
+  <si>
+    <t>Reset request(Bool)</t>
+  </si>
+  <si>
+    <t>RecBlockCount</t>
+  </si>
+  <si>
+    <t>SentBlockCount</t>
+  </si>
+  <si>
+    <t>COBID</t>
+  </si>
+  <si>
+    <t>0x63x</t>
+  </si>
+  <si>
+    <t>0x64x</t>
+  </si>
+  <si>
+    <t>ConfirmCodes:</t>
+  </si>
+  <si>
+    <t>eccNoConfirm,</t>
+  </si>
+  <si>
+    <t>eccAccept,</t>
+  </si>
+  <si>
+    <t>eccFlashErased,</t>
+  </si>
+  <si>
+    <t>eccInvalidBlockSize,</t>
+  </si>
+  <si>
+    <t>eccInvalidTotalSize,</t>
+  </si>
+  <si>
+    <t>eccBlockConfirm,</t>
+  </si>
+  <si>
+    <t>eccTotalTransferConfirm,</t>
+  </si>
+  <si>
+    <t>eccInvalidHwid,</t>
+  </si>
+  <si>
+    <t>eccErrorAborted</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Bootloader protocol for FW updates. Application code is transferred consecutivelly via standard CAN frames (8byte payload). CAN ID is 0x63x  for direction PC-&gt;Target,  and 0x64x for Target-&gt;PC. The Blocks are always same size </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1024B</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, except las block which may be shorter.  Blocks are saved to RAM, and once block is finished, they are stored to flash.   Max block count is 255.  Which means maximall transfer count is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>255kB!</t>
+    </r>
+  </si>
+  <si>
+    <t>Segment Num:</t>
+  </si>
+  <si>
+    <t>0-255</t>
+  </si>
+  <si>
+    <t>Block Num:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1752,6 +1933,15 @@
       <strike/>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -2044,7 +2234,7 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2119,6 +2309,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -14390,11 +14590,381 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C3:U30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:O10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" customWidth="1"/>
+    <col min="14" max="14" width="23.5703125" customWidth="1"/>
+    <col min="16" max="16" width="51.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:21" ht="15" customHeight="1">
+      <c r="C3" s="51" t="s">
+        <v>524</v>
+      </c>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="51"/>
+      <c r="O3" s="51"/>
+      <c r="P3" s="54"/>
+    </row>
+    <row r="4" spans="3:21">
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="51"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="54"/>
+    </row>
+    <row r="5" spans="3:21">
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="54"/>
+    </row>
+    <row r="6" spans="3:21">
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="51"/>
+      <c r="K6" s="51"/>
+      <c r="L6" s="51"/>
+      <c r="M6" s="51"/>
+      <c r="N6" s="51"/>
+      <c r="O6" s="51"/>
+      <c r="P6" s="54"/>
+    </row>
+    <row r="7" spans="3:21">
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="51"/>
+      <c r="M7" s="51"/>
+      <c r="N7" s="51"/>
+      <c r="O7" s="51"/>
+      <c r="P7" s="54"/>
+    </row>
+    <row r="8" spans="3:21">
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="51"/>
+      <c r="N8" s="51"/>
+      <c r="O8" s="51"/>
+      <c r="P8" s="54"/>
+    </row>
+    <row r="9" spans="3:21">
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="51"/>
+      <c r="K9" s="51"/>
+      <c r="L9" s="51"/>
+      <c r="M9" s="51"/>
+      <c r="N9" s="51"/>
+      <c r="O9" s="51"/>
+      <c r="P9" s="54"/>
+    </row>
+    <row r="10" spans="3:21">
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="51"/>
+      <c r="L10" s="51"/>
+      <c r="M10" s="51"/>
+      <c r="N10" s="51"/>
+      <c r="O10" s="51"/>
+      <c r="P10" s="54"/>
+    </row>
+    <row r="13" spans="3:21">
+      <c r="C13" t="s">
+        <v>511</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>481</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>482</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>483</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>484</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>485</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>486</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>487</v>
+      </c>
+      <c r="L13" s="15" t="s">
+        <v>488</v>
+      </c>
+      <c r="U13">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="14" spans="3:21">
+      <c r="D14" s="52" t="s">
+        <v>480</v>
+      </c>
+      <c r="E14" s="52" t="s">
+        <v>489</v>
+      </c>
+      <c r="F14" s="53" t="s">
+        <v>490</v>
+      </c>
+      <c r="G14" s="53"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="53"/>
+      <c r="L14" s="53"/>
+      <c r="S14">
+        <v>20001</v>
+      </c>
+    </row>
+    <row r="15" spans="3:21">
+      <c r="C15" t="s">
+        <v>512</v>
+      </c>
+      <c r="D15" t="s">
+        <v>495</v>
+      </c>
+      <c r="E15" t="s">
+        <v>491</v>
+      </c>
+      <c r="G15" s="49" t="s">
+        <v>503</v>
+      </c>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49" t="s">
+        <v>504</v>
+      </c>
+      <c r="J15" s="49"/>
+      <c r="K15" s="49"/>
+      <c r="L15" s="49"/>
+    </row>
+    <row r="16" spans="3:21">
+      <c r="C16" t="s">
+        <v>512</v>
+      </c>
+      <c r="D16" t="s">
+        <v>496</v>
+      </c>
+      <c r="E16" t="s">
+        <v>492</v>
+      </c>
+      <c r="F16" t="s">
+        <v>499</v>
+      </c>
+      <c r="G16" t="s">
+        <v>498</v>
+      </c>
+      <c r="H16" t="s">
+        <v>507</v>
+      </c>
+      <c r="I16" s="49" t="s">
+        <v>497</v>
+      </c>
+      <c r="J16" s="49"/>
+      <c r="K16" s="49"/>
+      <c r="L16" s="49"/>
+    </row>
+    <row r="17" spans="3:14">
+      <c r="C17" t="s">
+        <v>513</v>
+      </c>
+      <c r="D17" t="s">
+        <v>501</v>
+      </c>
+      <c r="E17" t="s">
+        <v>493</v>
+      </c>
+      <c r="F17" t="s">
+        <v>502</v>
+      </c>
+      <c r="G17" t="s">
+        <v>509</v>
+      </c>
+      <c r="I17" s="49" t="s">
+        <v>505</v>
+      </c>
+      <c r="J17" s="49"/>
+      <c r="K17" s="49"/>
+      <c r="L17" s="49"/>
+    </row>
+    <row r="18" spans="3:14">
+      <c r="C18" t="s">
+        <v>512</v>
+      </c>
+      <c r="D18" t="s">
+        <v>500</v>
+      </c>
+      <c r="E18" t="s">
+        <v>494</v>
+      </c>
+      <c r="G18" t="s">
+        <v>510</v>
+      </c>
+      <c r="H18" t="s">
+        <v>508</v>
+      </c>
+      <c r="I18" s="49" t="s">
+        <v>506</v>
+      </c>
+      <c r="J18" s="49"/>
+      <c r="K18" s="49"/>
+      <c r="L18" s="49"/>
+    </row>
+    <row r="22" spans="3:14">
+      <c r="M22" t="s">
+        <v>514</v>
+      </c>
+      <c r="N22" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="23" spans="3:14">
+      <c r="N23" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="24" spans="3:14">
+      <c r="N24" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="25" spans="3:14">
+      <c r="N25" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="26" spans="3:14">
+      <c r="F26" t="s">
+        <v>525</v>
+      </c>
+      <c r="G26" t="s">
+        <v>526</v>
+      </c>
+      <c r="N26" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="27" spans="3:14">
+      <c r="F27" t="s">
+        <v>527</v>
+      </c>
+      <c r="G27" t="s">
+        <v>526</v>
+      </c>
+      <c r="N27" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="28" spans="3:14">
+      <c r="N28" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="29" spans="3:14">
+      <c r="N29" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="30" spans="3:14">
+      <c r="N30" t="s">
+        <v>523</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="F14:L14"/>
+    <mergeCell ref="I15:L15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I16:L16"/>
+    <mergeCell ref="I18:L18"/>
+    <mergeCell ref="I17:L17"/>
+    <mergeCell ref="C3:O10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P352"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="C70" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>

</xml_diff>